<commit_message>
generated the maps and regressions for final project
</commit_message>
<xml_diff>
--- a/All dataset.xlsx
+++ b/All dataset.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alyssa/code/alyssageorgee/group23/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{602B1ECA-3CE0-9C46-8D3A-6A9C55A390A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6030EC59-0AEF-1947-9EF9-764A969D9637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{EF997A0B-C278-2140-872F-D8857E89B0A9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{EF997A0B-C278-2140-872F-D8857E89B0A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" refMode="R1C1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -147,13 +147,13 @@
     <t>Newham</t>
   </si>
   <si>
-    <t>Total Population, Estimated mid year population (2020)</t>
-  </si>
-  <si>
-    <t>Suicide counts (2020)</t>
-  </si>
-  <si>
-    <t>Suicide Rates (2020)</t>
+    <t>Total Population, Estimated mid year population (2019)</t>
+  </si>
+  <si>
+    <t>Suicide counts (2019)</t>
+  </si>
+  <si>
+    <t>Suicide Rates (2019)</t>
   </si>
 </sst>
 </file>
@@ -164,7 +164,7 @@
     <numFmt numFmtId="164" formatCode="_-[$£-809]* #,##0_-;\-[$£-809]* #,##0_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -200,6 +200,12 @@
       <color rgb="FF0B0C0C"/>
       <name val="Georgia"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -241,7 +247,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -271,6 +277,7 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -589,7 +596,7 @@
   <dimension ref="A1:AC34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -639,17 +646,17 @@
         <v>3.28</v>
       </c>
       <c r="D2" s="16">
-        <f>G2/F2</f>
-        <v>3.9075147090017976E-5</v>
+        <f>(G2/F2)*100</f>
+        <v>1.0140445165542768E-2</v>
       </c>
       <c r="E2" s="3">
         <v>35805</v>
       </c>
-      <c r="F2">
-        <v>179142</v>
+      <c r="F2" s="17">
+        <v>177507</v>
       </c>
       <c r="G2" s="2">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -677,17 +684,17 @@
         <v>3.16</v>
       </c>
       <c r="D3" s="16">
-        <f t="shared" ref="D3:D34" si="0">G3/F3</f>
-        <v>4.11773637736995E-5</v>
+        <f t="shared" ref="D3:D34" si="0">(G3/F3)*100</f>
+        <v>6.7233844482945879E-3</v>
       </c>
       <c r="E3" s="3">
         <v>27847</v>
       </c>
-      <c r="F3">
-        <v>388563</v>
+      <c r="F3" s="17">
+        <v>386710</v>
       </c>
       <c r="G3" s="2">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -715,16 +722,16 @@
       </c>
       <c r="D4" s="16">
         <f t="shared" si="0"/>
-        <v>2.1036687983843824E-5</v>
+        <v>6.9207067546097926E-3</v>
       </c>
       <c r="E4" s="3">
         <v>33659</v>
       </c>
-      <c r="F4">
-        <v>332752</v>
+      <c r="F4" s="17">
+        <v>332336</v>
       </c>
       <c r="G4" s="2">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -753,16 +760,16 @@
       </c>
       <c r="D5" s="16">
         <f t="shared" si="0"/>
-        <v>6.9912829740181854E-5</v>
+        <v>9.9439089874522602E-3</v>
       </c>
       <c r="E5" s="3">
         <v>29327</v>
       </c>
-      <c r="F5">
-        <v>271767</v>
+      <c r="F5" s="17">
+        <v>271523</v>
       </c>
       <c r="G5" s="2">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -791,16 +798,16 @@
       </c>
       <c r="D6" s="16">
         <f t="shared" si="0"/>
-        <v>7.3455739978433394E-5</v>
+        <v>9.6545993926379289E-3</v>
       </c>
       <c r="E6" s="3">
         <v>29918</v>
       </c>
-      <c r="F6">
-        <v>340341</v>
+      <c r="F6" s="17">
+        <v>341806</v>
       </c>
       <c r="G6" s="2">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -829,16 +836,16 @@
       </c>
       <c r="D7" s="16">
         <f t="shared" si="0"/>
-        <v>7.6730954417976528E-5</v>
+        <v>5.3939095056096658E-3</v>
       </c>
       <c r="E7" s="3">
         <v>29549</v>
       </c>
-      <c r="F7">
-        <v>260651</v>
+      <c r="F7" s="17">
+        <v>259552</v>
       </c>
       <c r="G7" s="2">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -867,16 +874,16 @@
       </c>
       <c r="D8" s="16">
         <f t="shared" si="0"/>
-        <v>6.1485887370798733E-5</v>
+        <v>8.7985140287418113E-3</v>
       </c>
       <c r="E8" s="3">
         <v>29222</v>
       </c>
-      <c r="F8">
-        <v>309014</v>
+      <c r="F8" s="17">
+        <v>306870</v>
       </c>
       <c r="G8" s="2">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -905,16 +912,16 @@
       </c>
       <c r="D9" s="16">
         <f t="shared" si="0"/>
-        <v>4.7555263178752311E-5</v>
+        <v>3.9815257206561551E-3</v>
       </c>
       <c r="E9" s="3">
         <v>31430</v>
       </c>
-      <c r="F9">
-        <v>252338</v>
+      <c r="F9" s="17">
+        <v>251160</v>
       </c>
       <c r="G9" s="2">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -943,16 +950,16 @@
       </c>
       <c r="D10" s="16">
         <f t="shared" si="0"/>
-        <v>4.27150933782452E-5</v>
+        <v>5.1550924732617484E-3</v>
       </c>
       <c r="E10" s="3">
         <v>27364</v>
       </c>
-      <c r="F10">
-        <v>327753</v>
+      <c r="F10" s="17">
+        <v>329771</v>
       </c>
       <c r="G10" s="2">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -981,16 +988,16 @@
       </c>
       <c r="D11" s="16">
         <f t="shared" si="0"/>
-        <v>4.5111990516457107E-5</v>
+        <v>5.5573939863944885E-3</v>
       </c>
       <c r="E11" s="3">
         <v>34163</v>
       </c>
-      <c r="F11">
-        <v>399007</v>
+      <c r="F11" s="17">
+        <v>395869</v>
       </c>
       <c r="G11" s="2">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -1020,16 +1027,16 @@
       </c>
       <c r="D12" s="16">
         <f t="shared" si="0"/>
-        <v>3.1073946670892724E-5</v>
+        <v>7.9746284129876034E-3</v>
       </c>
       <c r="E12" s="3">
         <v>30753</v>
       </c>
-      <c r="F12">
-        <v>321813</v>
+      <c r="F12" s="17">
+        <v>326034</v>
       </c>
       <c r="G12" s="2">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -1058,16 +1065,16 @@
       </c>
       <c r="D13" s="16">
         <f t="shared" si="0"/>
-        <v>7.1871181843464565E-5</v>
+        <v>1.0663990214220745E-2</v>
       </c>
       <c r="E13" s="3">
         <v>29192</v>
       </c>
-      <c r="F13">
-        <v>320017</v>
+      <c r="F13" s="17">
+        <v>318830</v>
       </c>
       <c r="G13" s="2">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -1096,16 +1103,16 @@
       </c>
       <c r="D14" s="16">
         <f t="shared" si="0"/>
-        <v>5.8956663576900781E-5</v>
+        <v>8.8280877054165222E-3</v>
       </c>
       <c r="E14" s="3">
         <v>26541</v>
       </c>
-      <c r="F14">
-        <v>305309</v>
+      <c r="F14" s="17">
+        <v>305842</v>
       </c>
       <c r="G14" s="2">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -1134,16 +1141,16 @@
       </c>
       <c r="D15" s="16">
         <f t="shared" si="0"/>
-        <v>4.1517606925136832E-5</v>
+        <v>7.2931354231060416E-3</v>
       </c>
       <c r="E15" s="3">
         <v>26672</v>
       </c>
-      <c r="F15">
-        <v>289034</v>
+      <c r="F15" s="17">
+        <v>287942</v>
       </c>
       <c r="G15" s="2">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -1172,16 +1179,16 @@
       </c>
       <c r="D16" s="16">
         <f t="shared" si="0"/>
-        <v>5.2145799655837725E-5</v>
+        <v>8.8607136096533444E-3</v>
       </c>
       <c r="E16" s="3">
         <v>28691</v>
       </c>
-      <c r="F16">
-        <v>249301</v>
+      <c r="F16" s="17">
+        <v>248287</v>
       </c>
       <c r="G16" s="2">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -1210,16 +1217,16 @@
       </c>
       <c r="D17" s="16">
         <f t="shared" si="0"/>
-        <v>5.3958937248753699E-5</v>
+        <v>4.1942036106101368E-3</v>
       </c>
       <c r="E17" s="3">
         <v>27853</v>
       </c>
-      <c r="F17">
-        <v>333587</v>
+      <c r="F17" s="17">
+        <v>333794</v>
       </c>
       <c r="G17" s="2">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -1248,13 +1255,13 @@
       </c>
       <c r="D18" s="16">
         <f t="shared" si="0"/>
-        <v>5.4163356683758216E-5</v>
+        <v>5.415494813761133E-3</v>
       </c>
       <c r="E18" s="3">
         <v>27946</v>
       </c>
-      <c r="F18">
-        <v>276940</v>
+      <c r="F18" s="17">
+        <v>276983</v>
       </c>
       <c r="G18" s="2">
         <v>15</v>
@@ -1286,16 +1293,16 @@
       </c>
       <c r="D19" s="16">
         <f t="shared" si="0"/>
-        <v>5.5617716532856987E-5</v>
+        <v>6.2249772296885551E-3</v>
       </c>
       <c r="E19" s="3">
         <v>29529</v>
       </c>
-      <c r="F19">
-        <v>305658</v>
+      <c r="F19" s="17">
+        <v>305222</v>
       </c>
       <c r="G19" s="2">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -1324,16 +1331,16 @@
       </c>
       <c r="D20" s="16">
         <f t="shared" si="0"/>
-        <v>8.6660536236140331E-5</v>
+        <v>1.1630780861550094E-2</v>
       </c>
       <c r="E20" s="3">
         <v>32398</v>
       </c>
-      <c r="F20">
-        <v>207707</v>
+      <c r="F20" s="17">
+        <v>206349</v>
       </c>
       <c r="G20" s="2">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -1362,16 +1369,16 @@
       </c>
       <c r="D21" s="16">
         <f t="shared" si="0"/>
-        <v>7.5703665571486966E-5</v>
+        <v>7.0700286336159652E-3</v>
       </c>
       <c r="E21" s="3">
         <v>41493</v>
       </c>
-      <c r="F21">
-        <v>198141</v>
+      <c r="F21" s="17">
+        <v>198019</v>
       </c>
       <c r="G21" s="2">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
@@ -1400,16 +1407,16 @@
       </c>
       <c r="D22" s="16">
         <f t="shared" si="0"/>
-        <v>8.7186914212920131E-5</v>
+        <v>4.3573406665762928E-3</v>
       </c>
       <c r="E22" s="3">
         <v>33003</v>
       </c>
-      <c r="F22">
-        <v>206453</v>
+      <c r="F22" s="17">
+        <v>206548</v>
       </c>
       <c r="G22" s="2">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
@@ -1438,16 +1445,16 @@
       </c>
       <c r="D23" s="16">
         <f t="shared" si="0"/>
-        <v>5.4589291400670238E-5</v>
+        <v>6.3698711162744146E-3</v>
       </c>
       <c r="E23" s="3">
         <v>37911</v>
       </c>
-      <c r="F23">
-        <v>329735</v>
+      <c r="F23" s="17">
+        <v>329677</v>
       </c>
       <c r="G23" s="2">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
@@ -1476,16 +1483,16 @@
       </c>
       <c r="D24" s="16">
         <f t="shared" si="0"/>
-        <v>1.0896569759839603E-4</v>
+        <v>8.6419686404562955E-3</v>
       </c>
       <c r="E24" s="3">
         <v>36527</v>
       </c>
-      <c r="F24">
-        <v>183544</v>
+      <c r="F24" s="17">
+        <v>185143</v>
       </c>
       <c r="G24" s="2">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
@@ -1514,16 +1521,16 @@
       </c>
       <c r="D25" s="16">
         <f t="shared" si="0"/>
-        <v>9.5624235006119956E-5</v>
+        <v>7.045456001127273E-3</v>
       </c>
       <c r="E25" s="3">
         <v>43315</v>
       </c>
-      <c r="F25">
-        <v>156864</v>
+      <c r="F25" s="17">
+        <v>156129</v>
       </c>
       <c r="G25" s="2">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
@@ -1549,16 +1556,16 @@
       </c>
       <c r="D26" s="16">
         <f t="shared" si="0"/>
-        <v>7.7821588449793964E-5</v>
+        <v>5.7401546780347246E-3</v>
       </c>
       <c r="E26" s="3">
         <v>40919</v>
       </c>
-      <c r="F26">
-        <v>269848</v>
+      <c r="F26" s="17">
+        <v>261317</v>
       </c>
       <c r="G26" s="2">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
@@ -1587,16 +1594,16 @@
       </c>
       <c r="D27" s="16">
         <f t="shared" si="0"/>
-        <v>9.6595543725582793E-5</v>
+        <v>7.036281288306071E-3</v>
       </c>
       <c r="E27" s="3">
         <v>36053</v>
       </c>
-      <c r="F27">
-        <v>279516</v>
+      <c r="F27" s="17">
+        <v>270029</v>
       </c>
       <c r="G27" s="2">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
@@ -1625,16 +1632,16 @@
       </c>
       <c r="D28" s="16">
         <f t="shared" si="0"/>
-        <v>4.8197271431971056E-5</v>
+        <v>5.2348765954826097E-3</v>
       </c>
       <c r="E28" s="3">
         <v>30760</v>
       </c>
-      <c r="F28">
-        <v>331969</v>
+      <c r="F28" s="17">
+        <v>324745</v>
       </c>
       <c r="G28" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
@@ -1663,16 +1670,16 @@
       </c>
       <c r="D29" s="16">
         <f t="shared" si="0"/>
-        <v>5.2395058742921628E-5</v>
+        <v>5.7739816139928323E-3</v>
       </c>
       <c r="E29" s="3">
         <v>33859</v>
       </c>
-      <c r="F29">
-        <v>248115</v>
+      <c r="F29" s="17">
+        <v>242467</v>
       </c>
       <c r="G29" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
@@ -1698,16 +1705,16 @@
       </c>
       <c r="D30" s="16">
         <f t="shared" si="0"/>
-        <v>9.2546121783577341E-5</v>
+        <v>4.6243597040409789E-3</v>
       </c>
       <c r="E30" s="3">
         <v>28043</v>
       </c>
-      <c r="F30">
-        <v>280941</v>
+      <c r="F30" s="17">
+        <v>281120</v>
       </c>
       <c r="G30" s="2">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
@@ -1736,16 +1743,16 @@
       </c>
       <c r="D31" s="16">
         <f t="shared" si="0"/>
-        <v>5.6315396253899842E-5</v>
+        <v>8.1891850644153844E-3</v>
       </c>
       <c r="E31" s="3">
         <v>29318</v>
       </c>
-      <c r="F31">
-        <v>266357</v>
+      <c r="F31" s="17">
+        <v>268647</v>
       </c>
       <c r="G31" s="2">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
@@ -1774,16 +1781,16 @@
       </c>
       <c r="D32" s="16">
         <f t="shared" si="0"/>
-        <v>6.4740222818958183E-5</v>
+        <v>3.1149648575328347E-3</v>
       </c>
       <c r="E32" s="3">
         <v>23143</v>
       </c>
-      <c r="F32">
-        <v>355266</v>
+      <c r="F32" s="17">
+        <v>353134</v>
       </c>
       <c r="G32" s="2">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
@@ -1812,16 +1819,16 @@
       </c>
       <c r="D33" s="16">
         <f t="shared" si="0"/>
-        <v>6.538786681425643E-5</v>
+        <v>6.1059810432773148E-3</v>
       </c>
       <c r="E33" s="3">
         <v>21953</v>
       </c>
-      <c r="F33">
-        <v>214107</v>
+      <c r="F33" s="17">
+        <v>212906</v>
       </c>
       <c r="G33" s="2">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
@@ -1851,16 +1858,16 @@
       </c>
       <c r="D34" s="16">
         <f t="shared" si="0"/>
-        <v>9.1424392027793011E-5</v>
+        <v>2.0574015019030965E-2</v>
       </c>
       <c r="E34" s="3">
         <v>45436</v>
       </c>
-      <c r="F34">
-        <v>10938</v>
+      <c r="F34" s="17">
+        <v>9721</v>
       </c>
       <c r="G34" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>

</xml_diff>

<commit_message>
regenerated the plots with mean instead of median
</commit_message>
<xml_diff>
--- a/All dataset.xlsx
+++ b/All dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alyssa/code/alyssageorgee/group23/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6030EC59-0AEF-1947-9EF9-764A969D9637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C50D2E59-F0B0-A74C-AD6B-0961C5A19394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{EF997A0B-C278-2140-872F-D8857E89B0A9}"/>
+    <workbookView xWindow="0" yWindow="540" windowWidth="28800" windowHeight="15800" xr2:uid="{EF997A0B-C278-2140-872F-D8857E89B0A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,9 +45,6 @@
     <t>Anxiety 2019, where 10 = very anxious</t>
   </si>
   <si>
-    <t>Median Household Income 2019 (annual)</t>
-  </si>
-  <si>
     <t>Kingston upon Thames</t>
   </si>
   <si>
@@ -154,14 +151,16 @@
   </si>
   <si>
     <t>Suicide Rates (2019)</t>
+  </si>
+  <si>
+    <t>Mean Household Income 2019 (annual)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_-[$£-809]* #,##0_-;\-[$£-809]* #,##0_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
+  <numFmts count="1">
     <numFmt numFmtId="165" formatCode="0.000%"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
@@ -253,7 +252,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -278,6 +276,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -595,8 +594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE956E78-015E-C346-AA3F-695F205998D1}">
   <dimension ref="A1:AC34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -609,7 +608,7 @@
     <col min="6" max="6" width="47.5" customWidth="1"/>
     <col min="7" max="7" width="20.33203125" customWidth="1"/>
     <col min="19" max="19" width="11.1640625" customWidth="1"/>
-    <col min="20" max="29" width="10.83203125" style="9"/>
+    <col min="20" max="29" width="10.83203125" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.2">
@@ -623,21 +622,21 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
         <v>39</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
       <c r="F1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" t="s">
         <v>37</v>
-      </c>
-      <c r="G1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:29" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1">
         <v>8.5000000000000006E-2</v>
@@ -645,14 +644,14 @@
       <c r="C2">
         <v>3.28</v>
       </c>
-      <c r="D2" s="16">
+      <c r="D2" s="15">
         <f>(G2/F2)*100</f>
         <v>1.0140445165542768E-2</v>
       </c>
-      <c r="E2" s="3">
-        <v>35805</v>
-      </c>
-      <c r="F2" s="17">
+      <c r="E2" s="17">
+        <v>50300</v>
+      </c>
+      <c r="F2" s="16">
         <v>177507</v>
       </c>
       <c r="G2" s="2">
@@ -660,22 +659,22 @@
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="10"/>
-      <c r="U2" s="11"/>
-      <c r="V2" s="11"/>
-      <c r="W2" s="11"/>
-      <c r="X2" s="11"/>
-      <c r="Y2" s="11"/>
-      <c r="Z2" s="11"/>
-      <c r="AA2" s="12"/>
-      <c r="AB2" s="13"/>
-      <c r="AC2" s="14"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="9"/>
+      <c r="U2" s="10"/>
+      <c r="V2" s="10"/>
+      <c r="W2" s="10"/>
+      <c r="X2" s="10"/>
+      <c r="Y2" s="10"/>
+      <c r="Z2" s="10"/>
+      <c r="AA2" s="11"/>
+      <c r="AB2" s="12"/>
+      <c r="AC2" s="13"/>
     </row>
     <row r="3" spans="1:29" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1">
         <v>8.3000000000000004E-2</v>
@@ -683,14 +682,14 @@
       <c r="C3">
         <v>3.16</v>
       </c>
-      <c r="D3" s="16">
+      <c r="D3" s="15">
         <f t="shared" ref="D3:D34" si="0">(G3/F3)*100</f>
         <v>6.7233844482945879E-3</v>
       </c>
-      <c r="E3" s="3">
-        <v>27847</v>
-      </c>
-      <c r="F3" s="17">
+      <c r="E3" s="17">
+        <v>36500</v>
+      </c>
+      <c r="F3" s="16">
         <v>386710</v>
       </c>
       <c r="G3" s="2">
@@ -698,21 +697,21 @@
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="10"/>
-      <c r="U3" s="11"/>
-      <c r="V3" s="11"/>
-      <c r="W3" s="11"/>
-      <c r="X3" s="11"/>
-      <c r="Y3" s="11"/>
-      <c r="Z3" s="11"/>
-      <c r="AA3" s="12"/>
-      <c r="AB3" s="13"/>
-      <c r="AC3" s="14"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="9"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="10"/>
+      <c r="W3" s="10"/>
+      <c r="X3" s="10"/>
+      <c r="Y3" s="10"/>
+      <c r="Z3" s="10"/>
+      <c r="AA3" s="11"/>
+      <c r="AB3" s="12"/>
+      <c r="AC3" s="13"/>
     </row>
     <row r="4" spans="1:29" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1">
         <v>0.10299999999999999</v>
@@ -720,14 +719,14 @@
       <c r="C4">
         <v>2.7</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D4" s="15">
         <f t="shared" si="0"/>
         <v>6.9207067546097926E-3</v>
       </c>
-      <c r="E4" s="3">
-        <v>33659</v>
-      </c>
-      <c r="F4" s="17">
+      <c r="E4" s="17">
+        <v>46600</v>
+      </c>
+      <c r="F4" s="16">
         <v>332336</v>
       </c>
       <c r="G4" s="2">
@@ -735,22 +734,22 @@
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
-      <c r="T4" s="10"/>
-      <c r="U4" s="11"/>
-      <c r="V4" s="11"/>
-      <c r="W4" s="11"/>
-      <c r="X4" s="11"/>
-      <c r="Y4" s="11"/>
-      <c r="Z4" s="11"/>
-      <c r="AA4" s="12"/>
-      <c r="AB4" s="13"/>
-      <c r="AC4" s="14"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
+      <c r="W4" s="10"/>
+      <c r="X4" s="10"/>
+      <c r="Y4" s="10"/>
+      <c r="Z4" s="10"/>
+      <c r="AA4" s="11"/>
+      <c r="AB4" s="12"/>
+      <c r="AC4" s="13"/>
     </row>
     <row r="5" spans="1:29" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1">
         <v>6.8000000000000005E-2</v>
@@ -758,14 +757,14 @@
       <c r="C5">
         <v>3.17</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="15">
         <f t="shared" si="0"/>
         <v>9.9439089874522602E-3</v>
       </c>
-      <c r="E5" s="3">
-        <v>29327</v>
-      </c>
-      <c r="F5" s="17">
+      <c r="E5" s="17">
+        <v>42000</v>
+      </c>
+      <c r="F5" s="16">
         <v>271523</v>
       </c>
       <c r="G5" s="2">
@@ -773,22 +772,22 @@
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
-      <c r="R5" s="4"/>
-      <c r="S5" s="4"/>
-      <c r="T5" s="10"/>
-      <c r="U5" s="11"/>
-      <c r="V5" s="11"/>
-      <c r="W5" s="11"/>
-      <c r="X5" s="11"/>
-      <c r="Y5" s="11"/>
-      <c r="Z5" s="11"/>
-      <c r="AA5" s="12"/>
-      <c r="AB5" s="13"/>
-      <c r="AC5" s="14"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="9"/>
+      <c r="U5" s="10"/>
+      <c r="V5" s="10"/>
+      <c r="W5" s="10"/>
+      <c r="X5" s="10"/>
+      <c r="Y5" s="10"/>
+      <c r="Z5" s="10"/>
+      <c r="AA5" s="11"/>
+      <c r="AB5" s="12"/>
+      <c r="AC5" s="13"/>
     </row>
     <row r="6" spans="1:29" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1">
         <v>6.0999999999999999E-2</v>
@@ -796,14 +795,14 @@
       <c r="C6">
         <v>3.27</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="15">
         <f t="shared" si="0"/>
         <v>9.6545993926379289E-3</v>
       </c>
-      <c r="E6" s="3">
-        <v>29918</v>
-      </c>
-      <c r="F6" s="17">
+      <c r="E6" s="17">
+        <v>39800</v>
+      </c>
+      <c r="F6" s="16">
         <v>341806</v>
       </c>
       <c r="G6" s="2">
@@ -811,22 +810,22 @@
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
-      <c r="T6" s="10"/>
-      <c r="U6" s="11"/>
-      <c r="V6" s="11"/>
-      <c r="W6" s="11"/>
-      <c r="X6" s="11"/>
-      <c r="Y6" s="11"/>
-      <c r="Z6" s="11"/>
-      <c r="AA6" s="12"/>
-      <c r="AB6" s="13"/>
-      <c r="AC6" s="14"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="10"/>
+      <c r="V6" s="10"/>
+      <c r="W6" s="10"/>
+      <c r="X6" s="10"/>
+      <c r="Y6" s="10"/>
+      <c r="Z6" s="10"/>
+      <c r="AA6" s="11"/>
+      <c r="AB6" s="12"/>
+      <c r="AC6" s="13"/>
     </row>
     <row r="7" spans="1:29" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1">
         <v>9.9000000000000005E-2</v>
@@ -834,14 +833,14 @@
       <c r="C7">
         <v>2.44</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D7" s="15">
         <f t="shared" si="0"/>
         <v>5.3939095056096658E-3</v>
       </c>
-      <c r="E7" s="3">
-        <v>29549</v>
-      </c>
-      <c r="F7" s="17">
+      <c r="E7" s="17">
+        <v>37100</v>
+      </c>
+      <c r="F7" s="16">
         <v>259552</v>
       </c>
       <c r="G7" s="2">
@@ -849,22 +848,22 @@
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
-      <c r="R7" s="4"/>
-      <c r="S7" s="4"/>
-      <c r="T7" s="10"/>
-      <c r="U7" s="11"/>
-      <c r="V7" s="11"/>
-      <c r="W7" s="11"/>
-      <c r="X7" s="11"/>
-      <c r="Y7" s="11"/>
-      <c r="Z7" s="11"/>
-      <c r="AA7" s="12"/>
-      <c r="AB7" s="13"/>
-      <c r="AC7" s="14"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="9"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="10"/>
+      <c r="W7" s="10"/>
+      <c r="X7" s="10"/>
+      <c r="Y7" s="10"/>
+      <c r="Z7" s="10"/>
+      <c r="AA7" s="11"/>
+      <c r="AB7" s="12"/>
+      <c r="AC7" s="13"/>
     </row>
     <row r="8" spans="1:29" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="1">
         <v>8.6999999999999994E-2</v>
@@ -872,14 +871,14 @@
       <c r="C8">
         <v>2.83</v>
       </c>
-      <c r="D8" s="16">
+      <c r="D8" s="15">
         <f t="shared" si="0"/>
         <v>8.7985140287418113E-3</v>
       </c>
-      <c r="E8" s="3">
-        <v>29222</v>
-      </c>
-      <c r="F8" s="17">
+      <c r="E8" s="17">
+        <v>36800</v>
+      </c>
+      <c r="F8" s="16">
         <v>306870</v>
       </c>
       <c r="G8" s="2">
@@ -887,22 +886,22 @@
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
-      <c r="R8" s="4"/>
-      <c r="S8" s="4"/>
-      <c r="T8" s="10"/>
-      <c r="U8" s="11"/>
-      <c r="V8" s="11"/>
-      <c r="W8" s="11"/>
-      <c r="X8" s="11"/>
-      <c r="Y8" s="11"/>
-      <c r="Z8" s="11"/>
-      <c r="AA8" s="12"/>
-      <c r="AB8" s="13"/>
-      <c r="AC8" s="14"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="10"/>
+      <c r="V8" s="10"/>
+      <c r="W8" s="10"/>
+      <c r="X8" s="10"/>
+      <c r="Y8" s="10"/>
+      <c r="Z8" s="10"/>
+      <c r="AA8" s="11"/>
+      <c r="AB8" s="12"/>
+      <c r="AC8" s="13"/>
     </row>
     <row r="9" spans="1:29" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="1">
         <v>7.0000000000000007E-2</v>
@@ -910,14 +909,14 @@
       <c r="C9">
         <v>3.15</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="15">
         <f t="shared" si="0"/>
         <v>3.9815257206561551E-3</v>
       </c>
-      <c r="E9" s="3">
-        <v>31430</v>
-      </c>
-      <c r="F9" s="17">
+      <c r="E9" s="17">
+        <v>39300</v>
+      </c>
+      <c r="F9" s="16">
         <v>251160</v>
       </c>
       <c r="G9" s="2">
@@ -925,22 +924,22 @@
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
-      <c r="R9" s="4"/>
-      <c r="S9" s="4"/>
-      <c r="T9" s="10"/>
-      <c r="U9" s="11"/>
-      <c r="V9" s="11"/>
-      <c r="W9" s="11"/>
-      <c r="X9" s="11"/>
-      <c r="Y9" s="11"/>
-      <c r="Z9" s="11"/>
-      <c r="AA9" s="12"/>
-      <c r="AB9" s="13"/>
-      <c r="AC9" s="14"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="10"/>
+      <c r="V9" s="10"/>
+      <c r="W9" s="10"/>
+      <c r="X9" s="10"/>
+      <c r="Y9" s="10"/>
+      <c r="Z9" s="10"/>
+      <c r="AA9" s="11"/>
+      <c r="AB9" s="12"/>
+      <c r="AC9" s="13"/>
     </row>
     <row r="10" spans="1:29" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="1">
         <v>6.6000000000000003E-2</v>
@@ -948,14 +947,14 @@
       <c r="C10">
         <v>3.04</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D10" s="15">
         <f t="shared" si="0"/>
         <v>5.1550924732617484E-3</v>
       </c>
-      <c r="E10" s="3">
-        <v>27364</v>
-      </c>
-      <c r="F10" s="17">
+      <c r="E10" s="17">
+        <v>36300</v>
+      </c>
+      <c r="F10" s="16">
         <v>329771</v>
       </c>
       <c r="G10" s="2">
@@ -963,37 +962,37 @@
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
-      <c r="R10" s="4"/>
-      <c r="S10" s="4"/>
-      <c r="T10" s="10"/>
-      <c r="U10" s="11"/>
-      <c r="V10" s="11"/>
-      <c r="W10" s="11"/>
-      <c r="X10" s="11"/>
-      <c r="Y10" s="11"/>
-      <c r="Z10" s="11"/>
-      <c r="AA10" s="12"/>
-      <c r="AB10" s="13"/>
-      <c r="AC10" s="14"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="9"/>
+      <c r="U10" s="10"/>
+      <c r="V10" s="10"/>
+      <c r="W10" s="10"/>
+      <c r="X10" s="10"/>
+      <c r="Y10" s="10"/>
+      <c r="Z10" s="10"/>
+      <c r="AA10" s="11"/>
+      <c r="AB10" s="12"/>
+      <c r="AC10" s="13"/>
     </row>
     <row r="11" spans="1:29" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="5">
+        <v>14</v>
+      </c>
+      <c r="B11" s="4">
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="C11">
         <v>2.85</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="15">
         <f t="shared" si="0"/>
         <v>5.5573939863944885E-3</v>
       </c>
-      <c r="E11" s="3">
-        <v>34163</v>
-      </c>
-      <c r="F11" s="17">
+      <c r="E11" s="17">
+        <v>51600</v>
+      </c>
+      <c r="F11" s="16">
         <v>395869</v>
       </c>
       <c r="G11" s="2">
@@ -1001,23 +1000,23 @@
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
-      <c r="K11" s="6"/>
-      <c r="R11" s="4"/>
-      <c r="S11" s="4"/>
-      <c r="T11" s="15"/>
-      <c r="U11" s="12"/>
-      <c r="V11" s="12"/>
-      <c r="W11" s="12"/>
-      <c r="X11" s="12"/>
-      <c r="Y11" s="12"/>
-      <c r="Z11" s="12"/>
-      <c r="AA11" s="12"/>
-      <c r="AB11" s="13"/>
-      <c r="AC11" s="14"/>
+      <c r="K11" s="5"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="14"/>
+      <c r="U11" s="11"/>
+      <c r="V11" s="11"/>
+      <c r="W11" s="11"/>
+      <c r="X11" s="11"/>
+      <c r="Y11" s="11"/>
+      <c r="Z11" s="11"/>
+      <c r="AA11" s="11"/>
+      <c r="AB11" s="12"/>
+      <c r="AC11" s="13"/>
     </row>
     <row r="12" spans="1:29" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" s="1">
         <v>8.7999999999999995E-2</v>
@@ -1025,14 +1024,14 @@
       <c r="C12">
         <v>3.71</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D12" s="15">
         <f t="shared" si="0"/>
         <v>7.9746284129876034E-3</v>
       </c>
-      <c r="E12" s="3">
-        <v>30753</v>
-      </c>
-      <c r="F12" s="17">
+      <c r="E12" s="17">
+        <v>47500</v>
+      </c>
+      <c r="F12" s="16">
         <v>326034</v>
       </c>
       <c r="G12" s="2">
@@ -1040,22 +1039,22 @@
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
-      <c r="R12" s="4"/>
-      <c r="S12" s="4"/>
-      <c r="T12" s="10"/>
-      <c r="U12" s="11"/>
-      <c r="V12" s="11"/>
-      <c r="W12" s="11"/>
-      <c r="X12" s="11"/>
-      <c r="Y12" s="11"/>
-      <c r="Z12" s="11"/>
-      <c r="AA12" s="12"/>
-      <c r="AB12" s="13"/>
-      <c r="AC12" s="14"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="10"/>
+      <c r="V12" s="10"/>
+      <c r="W12" s="10"/>
+      <c r="X12" s="10"/>
+      <c r="Y12" s="10"/>
+      <c r="Z12" s="10"/>
+      <c r="AA12" s="11"/>
+      <c r="AB12" s="12"/>
+      <c r="AC12" s="13"/>
     </row>
     <row r="13" spans="1:29" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" s="1">
         <v>9.0999999999999998E-2</v>
@@ -1063,14 +1062,14 @@
       <c r="C13">
         <v>3.04</v>
       </c>
-      <c r="D13" s="16">
+      <c r="D13" s="15">
         <f t="shared" si="0"/>
         <v>1.0663990214220745E-2</v>
       </c>
-      <c r="E13" s="3">
-        <v>29192</v>
-      </c>
-      <c r="F13" s="17">
+      <c r="E13" s="17">
+        <v>49400</v>
+      </c>
+      <c r="F13" s="16">
         <v>318830</v>
       </c>
       <c r="G13" s="2">
@@ -1078,22 +1077,22 @@
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
-      <c r="R13" s="4"/>
-      <c r="S13" s="4"/>
-      <c r="T13" s="10"/>
-      <c r="U13" s="11"/>
-      <c r="V13" s="11"/>
-      <c r="W13" s="11"/>
-      <c r="X13" s="11"/>
-      <c r="Y13" s="11"/>
-      <c r="Z13" s="11"/>
-      <c r="AA13" s="12"/>
-      <c r="AB13" s="13"/>
-      <c r="AC13" s="14"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="9"/>
+      <c r="U13" s="10"/>
+      <c r="V13" s="10"/>
+      <c r="W13" s="10"/>
+      <c r="X13" s="10"/>
+      <c r="Y13" s="10"/>
+      <c r="Z13" s="10"/>
+      <c r="AA13" s="11"/>
+      <c r="AB13" s="12"/>
+      <c r="AC13" s="13"/>
     </row>
     <row r="14" spans="1:29" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" s="1">
         <v>9.2999999999999999E-2</v>
@@ -1101,14 +1100,14 @@
       <c r="C14">
         <v>3.32</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D14" s="15">
         <f t="shared" si="0"/>
         <v>8.8280877054165222E-3</v>
       </c>
-      <c r="E14" s="3">
-        <v>26541</v>
-      </c>
-      <c r="F14" s="17">
+      <c r="E14" s="17">
+        <v>38000</v>
+      </c>
+      <c r="F14" s="16">
         <v>305842</v>
       </c>
       <c r="G14" s="2">
@@ -1116,22 +1115,22 @@
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
-      <c r="R14" s="4"/>
-      <c r="S14" s="4"/>
-      <c r="T14" s="10"/>
-      <c r="U14" s="11"/>
-      <c r="V14" s="11"/>
-      <c r="W14" s="11"/>
-      <c r="X14" s="11"/>
-      <c r="Y14" s="11"/>
-      <c r="Z14" s="11"/>
-      <c r="AA14" s="12"/>
-      <c r="AB14" s="13"/>
-      <c r="AC14" s="14"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+      <c r="T14" s="9"/>
+      <c r="U14" s="10"/>
+      <c r="V14" s="10"/>
+      <c r="W14" s="10"/>
+      <c r="X14" s="10"/>
+      <c r="Y14" s="10"/>
+      <c r="Z14" s="10"/>
+      <c r="AA14" s="11"/>
+      <c r="AB14" s="12"/>
+      <c r="AC14" s="13"/>
     </row>
     <row r="15" spans="1:29" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" s="1">
         <v>6.9000000000000006E-2</v>
@@ -1139,14 +1138,14 @@
       <c r="C15">
         <v>2.63</v>
       </c>
-      <c r="D15" s="16">
+      <c r="D15" s="15">
         <f t="shared" si="0"/>
         <v>7.2931354231060416E-3</v>
       </c>
-      <c r="E15" s="3">
-        <v>26672</v>
-      </c>
-      <c r="F15" s="17">
+      <c r="E15" s="17">
+        <v>41300</v>
+      </c>
+      <c r="F15" s="16">
         <v>287942</v>
       </c>
       <c r="G15" s="2">
@@ -1154,22 +1153,22 @@
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
-      <c r="R15" s="4"/>
-      <c r="S15" s="4"/>
-      <c r="T15" s="10"/>
-      <c r="U15" s="11"/>
-      <c r="V15" s="11"/>
-      <c r="W15" s="11"/>
-      <c r="X15" s="11"/>
-      <c r="Y15" s="11"/>
-      <c r="Z15" s="11"/>
-      <c r="AA15" s="12"/>
-      <c r="AB15" s="13"/>
-      <c r="AC15" s="14"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3"/>
+      <c r="T15" s="9"/>
+      <c r="U15" s="10"/>
+      <c r="V15" s="10"/>
+      <c r="W15" s="10"/>
+      <c r="X15" s="10"/>
+      <c r="Y15" s="10"/>
+      <c r="Z15" s="10"/>
+      <c r="AA15" s="11"/>
+      <c r="AB15" s="12"/>
+      <c r="AC15" s="13"/>
     </row>
     <row r="16" spans="1:29" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B16" s="1">
         <v>9.4E-2</v>
@@ -1177,14 +1176,14 @@
       <c r="C16">
         <v>2.78</v>
       </c>
-      <c r="D16" s="16">
+      <c r="D16" s="15">
         <f t="shared" si="0"/>
         <v>8.8607136096533444E-3</v>
       </c>
-      <c r="E16" s="3">
-        <v>28691</v>
-      </c>
-      <c r="F16" s="17">
+      <c r="E16" s="17">
+        <v>34600</v>
+      </c>
+      <c r="F16" s="16">
         <v>248287</v>
       </c>
       <c r="G16" s="2">
@@ -1192,22 +1191,22 @@
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
-      <c r="R16" s="4"/>
-      <c r="S16" s="4"/>
-      <c r="T16" s="10"/>
-      <c r="U16" s="11"/>
-      <c r="V16" s="11"/>
-      <c r="W16" s="11"/>
-      <c r="X16" s="11"/>
-      <c r="Y16" s="11"/>
-      <c r="Z16" s="11"/>
-      <c r="AA16" s="12"/>
-      <c r="AB16" s="13"/>
-      <c r="AC16" s="14"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="3"/>
+      <c r="T16" s="9"/>
+      <c r="U16" s="10"/>
+      <c r="V16" s="10"/>
+      <c r="W16" s="10"/>
+      <c r="X16" s="10"/>
+      <c r="Y16" s="10"/>
+      <c r="Z16" s="10"/>
+      <c r="AA16" s="11"/>
+      <c r="AB16" s="12"/>
+      <c r="AC16" s="13"/>
     </row>
     <row r="17" spans="1:29" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B17" s="1">
         <v>0.113</v>
@@ -1215,14 +1214,14 @@
       <c r="C17">
         <v>3.23</v>
       </c>
-      <c r="D17" s="16">
+      <c r="D17" s="15">
         <f t="shared" si="0"/>
         <v>4.1942036106101368E-3</v>
       </c>
-      <c r="E17" s="3">
-        <v>27853</v>
-      </c>
-      <c r="F17" s="17">
+      <c r="E17" s="17">
+        <v>37200</v>
+      </c>
+      <c r="F17" s="16">
         <v>333794</v>
       </c>
       <c r="G17" s="2">
@@ -1230,22 +1229,22 @@
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
-      <c r="R17" s="4"/>
-      <c r="S17" s="4"/>
-      <c r="T17" s="10"/>
-      <c r="U17" s="11"/>
-      <c r="V17" s="11"/>
-      <c r="W17" s="11"/>
-      <c r="X17" s="11"/>
-      <c r="Y17" s="11"/>
-      <c r="Z17" s="11"/>
-      <c r="AA17" s="12"/>
-      <c r="AB17" s="13"/>
-      <c r="AC17" s="14"/>
+      <c r="R17" s="3"/>
+      <c r="S17" s="3"/>
+      <c r="T17" s="9"/>
+      <c r="U17" s="10"/>
+      <c r="V17" s="10"/>
+      <c r="W17" s="10"/>
+      <c r="X17" s="10"/>
+      <c r="Y17" s="10"/>
+      <c r="Z17" s="10"/>
+      <c r="AA17" s="11"/>
+      <c r="AB17" s="12"/>
+      <c r="AC17" s="13"/>
     </row>
     <row r="18" spans="1:29" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18" s="1">
         <v>7.8E-2</v>
@@ -1253,14 +1252,14 @@
       <c r="C18">
         <v>2.94</v>
       </c>
-      <c r="D18" s="16">
+      <c r="D18" s="15">
         <f t="shared" si="0"/>
         <v>5.415494813761133E-3</v>
       </c>
-      <c r="E18" s="3">
-        <v>27946</v>
-      </c>
-      <c r="F18" s="17">
+      <c r="E18" s="17">
+        <v>33700</v>
+      </c>
+      <c r="F18" s="16">
         <v>276983</v>
       </c>
       <c r="G18" s="2">
@@ -1268,22 +1267,22 @@
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
-      <c r="R18" s="4"/>
-      <c r="S18" s="4"/>
-      <c r="T18" s="10"/>
-      <c r="U18" s="11"/>
-      <c r="V18" s="11"/>
-      <c r="W18" s="11"/>
-      <c r="X18" s="11"/>
-      <c r="Y18" s="11"/>
-      <c r="Z18" s="11"/>
-      <c r="AA18" s="12"/>
-      <c r="AB18" s="13"/>
-      <c r="AC18" s="14"/>
+      <c r="R18" s="3"/>
+      <c r="S18" s="3"/>
+      <c r="T18" s="9"/>
+      <c r="U18" s="10"/>
+      <c r="V18" s="10"/>
+      <c r="W18" s="10"/>
+      <c r="X18" s="10"/>
+      <c r="Y18" s="10"/>
+      <c r="Z18" s="10"/>
+      <c r="AA18" s="11"/>
+      <c r="AB18" s="12"/>
+      <c r="AC18" s="13"/>
     </row>
     <row r="19" spans="1:29" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" s="1">
         <v>6.3E-2</v>
@@ -1291,14 +1290,14 @@
       <c r="C19">
         <v>3.07</v>
       </c>
-      <c r="D19" s="16">
+      <c r="D19" s="15">
         <f t="shared" si="0"/>
         <v>6.2249772296885551E-3</v>
       </c>
-      <c r="E19" s="3">
-        <v>29529</v>
-      </c>
-      <c r="F19" s="17">
+      <c r="E19" s="17">
+        <v>37100</v>
+      </c>
+      <c r="F19" s="16">
         <v>305222</v>
       </c>
       <c r="G19" s="2">
@@ -1306,22 +1305,22 @@
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
-      <c r="R19" s="4"/>
-      <c r="S19" s="4"/>
-      <c r="T19" s="10"/>
-      <c r="U19" s="11"/>
-      <c r="V19" s="11"/>
-      <c r="W19" s="11"/>
-      <c r="X19" s="11"/>
-      <c r="Y19" s="11"/>
-      <c r="Z19" s="11"/>
-      <c r="AA19" s="12"/>
-      <c r="AB19" s="13"/>
-      <c r="AC19" s="14"/>
+      <c r="R19" s="3"/>
+      <c r="S19" s="3"/>
+      <c r="T19" s="9"/>
+      <c r="U19" s="10"/>
+      <c r="V19" s="10"/>
+      <c r="W19" s="10"/>
+      <c r="X19" s="10"/>
+      <c r="Y19" s="10"/>
+      <c r="Z19" s="10"/>
+      <c r="AA19" s="11"/>
+      <c r="AB19" s="12"/>
+      <c r="AC19" s="13"/>
     </row>
     <row r="20" spans="1:29" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20" s="1">
         <v>0.106</v>
@@ -1329,14 +1328,14 @@
       <c r="C20">
         <v>3.38</v>
       </c>
-      <c r="D20" s="16">
+      <c r="D20" s="15">
         <f t="shared" si="0"/>
         <v>1.1630780861550094E-2</v>
       </c>
-      <c r="E20" s="3">
-        <v>32398</v>
-      </c>
-      <c r="F20" s="17">
+      <c r="E20" s="17">
+        <v>38500</v>
+      </c>
+      <c r="F20" s="16">
         <v>206349</v>
       </c>
       <c r="G20" s="2">
@@ -1344,22 +1343,22 @@
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
-      <c r="R20" s="4"/>
-      <c r="S20" s="4"/>
-      <c r="T20" s="10"/>
-      <c r="U20" s="11"/>
-      <c r="V20" s="11"/>
-      <c r="W20" s="11"/>
-      <c r="X20" s="11"/>
-      <c r="Y20" s="11"/>
-      <c r="Z20" s="11"/>
-      <c r="AA20" s="12"/>
-      <c r="AB20" s="13"/>
-      <c r="AC20" s="14"/>
+      <c r="R20" s="3"/>
+      <c r="S20" s="3"/>
+      <c r="T20" s="9"/>
+      <c r="U20" s="10"/>
+      <c r="V20" s="10"/>
+      <c r="W20" s="10"/>
+      <c r="X20" s="10"/>
+      <c r="Y20" s="10"/>
+      <c r="Z20" s="10"/>
+      <c r="AA20" s="11"/>
+      <c r="AB20" s="12"/>
+      <c r="AC20" s="13"/>
     </row>
     <row r="21" spans="1:29" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B21" s="1">
         <v>7.0999999999999994E-2</v>
@@ -1367,14 +1366,14 @@
       <c r="C21">
         <v>3.28</v>
       </c>
-      <c r="D21" s="16">
+      <c r="D21" s="15">
         <f t="shared" si="0"/>
         <v>7.0700286336159652E-3</v>
       </c>
-      <c r="E21" s="3">
-        <v>41493</v>
-      </c>
-      <c r="F21" s="17">
+      <c r="E21" s="17">
+        <v>73800</v>
+      </c>
+      <c r="F21" s="16">
         <v>198019</v>
       </c>
       <c r="G21" s="2">
@@ -1382,22 +1381,22 @@
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
-      <c r="R21" s="4"/>
-      <c r="S21" s="4"/>
-      <c r="T21" s="10"/>
-      <c r="U21" s="11"/>
-      <c r="V21" s="11"/>
-      <c r="W21" s="11"/>
-      <c r="X21" s="11"/>
-      <c r="Y21" s="11"/>
-      <c r="Z21" s="11"/>
-      <c r="AA21" s="12"/>
-      <c r="AB21" s="13"/>
-      <c r="AC21" s="14"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="3"/>
+      <c r="T21" s="9"/>
+      <c r="U21" s="10"/>
+      <c r="V21" s="10"/>
+      <c r="W21" s="10"/>
+      <c r="X21" s="10"/>
+      <c r="Y21" s="10"/>
+      <c r="Z21" s="10"/>
+      <c r="AA21" s="11"/>
+      <c r="AB21" s="12"/>
+      <c r="AC21" s="13"/>
     </row>
     <row r="22" spans="1:29" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" s="1">
         <v>8.5999999999999993E-2</v>
@@ -1405,14 +1404,14 @@
       <c r="C22">
         <v>3.04</v>
       </c>
-      <c r="D22" s="16">
+      <c r="D22" s="15">
         <f t="shared" si="0"/>
         <v>4.3573406665762928E-3</v>
       </c>
-      <c r="E22" s="3">
-        <v>33003</v>
-      </c>
-      <c r="F22" s="17">
+      <c r="E22" s="17">
+        <v>56300</v>
+      </c>
+      <c r="F22" s="16">
         <v>206548</v>
       </c>
       <c r="G22" s="2">
@@ -1420,22 +1419,22 @@
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
-      <c r="R22" s="4"/>
-      <c r="S22" s="4"/>
-      <c r="T22" s="10"/>
-      <c r="U22" s="11"/>
-      <c r="V22" s="11"/>
-      <c r="W22" s="11"/>
-      <c r="X22" s="11"/>
-      <c r="Y22" s="11"/>
-      <c r="Z22" s="11"/>
-      <c r="AA22" s="12"/>
-      <c r="AB22" s="13"/>
-      <c r="AC22" s="14"/>
+      <c r="R22" s="3"/>
+      <c r="S22" s="3"/>
+      <c r="T22" s="9"/>
+      <c r="U22" s="10"/>
+      <c r="V22" s="10"/>
+      <c r="W22" s="10"/>
+      <c r="X22" s="10"/>
+      <c r="Y22" s="10"/>
+      <c r="Z22" s="10"/>
+      <c r="AA22" s="11"/>
+      <c r="AB22" s="12"/>
+      <c r="AC22" s="13"/>
     </row>
     <row r="23" spans="1:29" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B23" s="1">
         <v>7.8E-2</v>
@@ -1443,14 +1442,14 @@
       <c r="C23">
         <v>3.26</v>
       </c>
-      <c r="D23" s="16">
+      <c r="D23" s="15">
         <f t="shared" si="0"/>
         <v>6.3698711162744146E-3</v>
       </c>
-      <c r="E23" s="3">
-        <v>37911</v>
-      </c>
-      <c r="F23" s="17">
+      <c r="E23" s="17">
+        <v>70400</v>
+      </c>
+      <c r="F23" s="16">
         <v>329677</v>
       </c>
       <c r="G23" s="2">
@@ -1458,22 +1457,22 @@
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
-      <c r="R23" s="4"/>
-      <c r="S23" s="4"/>
-      <c r="T23" s="10"/>
-      <c r="U23" s="11"/>
-      <c r="V23" s="11"/>
-      <c r="W23" s="11"/>
-      <c r="X23" s="11"/>
-      <c r="Y23" s="11"/>
-      <c r="Z23" s="11"/>
-      <c r="AA23" s="12"/>
-      <c r="AB23" s="13"/>
-      <c r="AC23" s="14"/>
+      <c r="R23" s="3"/>
+      <c r="S23" s="3"/>
+      <c r="T23" s="9"/>
+      <c r="U23" s="10"/>
+      <c r="V23" s="10"/>
+      <c r="W23" s="10"/>
+      <c r="X23" s="10"/>
+      <c r="Y23" s="10"/>
+      <c r="Z23" s="10"/>
+      <c r="AA23" s="11"/>
+      <c r="AB23" s="12"/>
+      <c r="AC23" s="13"/>
     </row>
     <row r="24" spans="1:29" ht="18" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24" s="1">
         <v>6.6000000000000003E-2</v>
@@ -1481,14 +1480,14 @@
       <c r="C24">
         <v>3.23</v>
       </c>
-      <c r="D24" s="16">
+      <c r="D24" s="15">
         <f t="shared" si="0"/>
         <v>8.6419686404562955E-3</v>
       </c>
-      <c r="E24" s="3">
-        <v>36527</v>
-      </c>
-      <c r="F24" s="17">
+      <c r="E24" s="17">
+        <v>72600</v>
+      </c>
+      <c r="F24" s="16">
         <v>185143</v>
       </c>
       <c r="G24" s="2">
@@ -1496,22 +1495,22 @@
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
-      <c r="R24" s="4"/>
-      <c r="S24" s="4"/>
-      <c r="T24" s="10"/>
-      <c r="U24" s="11"/>
-      <c r="V24" s="11"/>
-      <c r="W24" s="11"/>
-      <c r="X24" s="11"/>
-      <c r="Y24" s="11"/>
-      <c r="Z24" s="11"/>
-      <c r="AA24" s="12"/>
-      <c r="AB24" s="13"/>
-      <c r="AC24" s="14"/>
+      <c r="R24" s="3"/>
+      <c r="S24" s="3"/>
+      <c r="T24" s="9"/>
+      <c r="U24" s="10"/>
+      <c r="V24" s="10"/>
+      <c r="W24" s="10"/>
+      <c r="X24" s="10"/>
+      <c r="Y24" s="10"/>
+      <c r="Z24" s="10"/>
+      <c r="AA24" s="11"/>
+      <c r="AB24" s="12"/>
+      <c r="AC24" s="13"/>
     </row>
     <row r="25" spans="1:29" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25" s="1">
         <v>8.3000000000000004E-2</v>
@@ -1519,14 +1518,14 @@
       <c r="C25">
         <v>3.35</v>
       </c>
-      <c r="D25" s="16">
+      <c r="D25" s="15">
         <f t="shared" si="0"/>
         <v>7.045456001127273E-3</v>
       </c>
-      <c r="E25" s="3">
-        <v>43315</v>
-      </c>
-      <c r="F25" s="17">
+      <c r="E25" s="17">
+        <v>173000</v>
+      </c>
+      <c r="F25" s="16">
         <v>156129</v>
       </c>
       <c r="G25" s="2">
@@ -1534,34 +1533,34 @@
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
-      <c r="R25" s="4"/>
-      <c r="S25" s="4"/>
-      <c r="T25" s="10"/>
-      <c r="U25" s="11"/>
-      <c r="V25" s="11"/>
-      <c r="W25" s="11"/>
-      <c r="X25" s="11"/>
-      <c r="Y25" s="11"/>
-      <c r="Z25" s="11"/>
-      <c r="AA25" s="12"/>
-      <c r="AB25" s="13"/>
-      <c r="AC25" s="14"/>
+      <c r="R25" s="3"/>
+      <c r="S25" s="3"/>
+      <c r="T25" s="9"/>
+      <c r="U25" s="10"/>
+      <c r="V25" s="10"/>
+      <c r="W25" s="10"/>
+      <c r="X25" s="10"/>
+      <c r="Y25" s="10"/>
+      <c r="Z25" s="10"/>
+      <c r="AA25" s="11"/>
+      <c r="AB25" s="12"/>
+      <c r="AC25" s="13"/>
     </row>
     <row r="26" spans="1:29" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C26">
         <v>2.88</v>
       </c>
-      <c r="D26" s="16">
+      <c r="D26" s="15">
         <f t="shared" si="0"/>
         <v>5.7401546780347246E-3</v>
       </c>
-      <c r="E26" s="3">
-        <v>40919</v>
-      </c>
-      <c r="F26" s="17">
+      <c r="E26" s="17">
+        <v>120000</v>
+      </c>
+      <c r="F26" s="16">
         <v>261317</v>
       </c>
       <c r="G26" s="2">
@@ -1569,22 +1568,22 @@
       </c>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
-      <c r="R26" s="4"/>
-      <c r="S26" s="4"/>
-      <c r="T26" s="10"/>
-      <c r="U26" s="11"/>
-      <c r="V26" s="11"/>
-      <c r="W26" s="11"/>
-      <c r="X26" s="11"/>
-      <c r="Y26" s="11"/>
-      <c r="Z26" s="11"/>
-      <c r="AA26" s="12"/>
-      <c r="AB26" s="13"/>
-      <c r="AC26" s="14"/>
+      <c r="R26" s="3"/>
+      <c r="S26" s="3"/>
+      <c r="T26" s="9"/>
+      <c r="U26" s="10"/>
+      <c r="V26" s="10"/>
+      <c r="W26" s="10"/>
+      <c r="X26" s="10"/>
+      <c r="Y26" s="10"/>
+      <c r="Z26" s="10"/>
+      <c r="AA26" s="11"/>
+      <c r="AB26" s="12"/>
+      <c r="AC26" s="13"/>
     </row>
     <row r="27" spans="1:29" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B27" s="1">
         <v>9.1999999999999998E-2</v>
@@ -1592,14 +1591,14 @@
       <c r="C27">
         <v>3.13</v>
       </c>
-      <c r="D27" s="16">
+      <c r="D27" s="15">
         <f t="shared" si="0"/>
         <v>7.036281288306071E-3</v>
       </c>
-      <c r="E27" s="3">
-        <v>36053</v>
-      </c>
-      <c r="F27" s="17">
+      <c r="E27" s="17">
+        <v>87400</v>
+      </c>
+      <c r="F27" s="16">
         <v>270029</v>
       </c>
       <c r="G27" s="2">
@@ -1607,22 +1606,22 @@
       </c>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
-      <c r="R27" s="4"/>
-      <c r="S27" s="4"/>
-      <c r="T27" s="10"/>
-      <c r="U27" s="11"/>
-      <c r="V27" s="11"/>
-      <c r="W27" s="11"/>
-      <c r="X27" s="11"/>
-      <c r="Y27" s="11"/>
-      <c r="Z27" s="11"/>
-      <c r="AA27" s="12"/>
-      <c r="AB27" s="13"/>
-      <c r="AC27" s="14"/>
+      <c r="R27" s="3"/>
+      <c r="S27" s="3"/>
+      <c r="T27" s="9"/>
+      <c r="U27" s="10"/>
+      <c r="V27" s="10"/>
+      <c r="W27" s="10"/>
+      <c r="X27" s="10"/>
+      <c r="Y27" s="10"/>
+      <c r="Z27" s="10"/>
+      <c r="AA27" s="11"/>
+      <c r="AB27" s="12"/>
+      <c r="AC27" s="13"/>
     </row>
     <row r="28" spans="1:29" ht="18" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B28" s="1">
         <v>8.4000000000000005E-2</v>
@@ -1630,14 +1629,14 @@
       <c r="C28">
         <v>3.68</v>
       </c>
-      <c r="D28" s="16">
+      <c r="D28" s="15">
         <f t="shared" si="0"/>
         <v>5.2348765954826097E-3</v>
       </c>
-      <c r="E28" s="3">
-        <v>30760</v>
-      </c>
-      <c r="F28" s="17">
+      <c r="E28" s="17">
+        <v>49300</v>
+      </c>
+      <c r="F28" s="16">
         <v>324745</v>
       </c>
       <c r="G28" s="2">
@@ -1645,22 +1644,22 @@
       </c>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
-      <c r="R28" s="4"/>
-      <c r="S28" s="4"/>
-      <c r="T28" s="10"/>
-      <c r="U28" s="11"/>
-      <c r="V28" s="11"/>
-      <c r="W28" s="11"/>
-      <c r="X28" s="11"/>
-      <c r="Y28" s="11"/>
-      <c r="Z28" s="11"/>
-      <c r="AA28" s="12"/>
-      <c r="AB28" s="13"/>
-      <c r="AC28" s="14"/>
+      <c r="R28" s="3"/>
+      <c r="S28" s="3"/>
+      <c r="T28" s="9"/>
+      <c r="U28" s="10"/>
+      <c r="V28" s="10"/>
+      <c r="W28" s="10"/>
+      <c r="X28" s="10"/>
+      <c r="Y28" s="10"/>
+      <c r="Z28" s="10"/>
+      <c r="AA28" s="11"/>
+      <c r="AB28" s="12"/>
+      <c r="AC28" s="13"/>
     </row>
     <row r="29" spans="1:29" ht="18" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B29" s="1">
         <v>0.104</v>
@@ -1668,14 +1667,14 @@
       <c r="C29">
         <v>3.34</v>
       </c>
-      <c r="D29" s="16">
+      <c r="D29" s="15">
         <f t="shared" si="0"/>
         <v>5.7739816139928323E-3</v>
       </c>
-      <c r="E29" s="3">
-        <v>33859</v>
-      </c>
-      <c r="F29" s="17">
+      <c r="E29" s="17">
+        <v>63900</v>
+      </c>
+      <c r="F29" s="16">
         <v>242467</v>
       </c>
       <c r="G29" s="2">
@@ -1683,34 +1682,34 @@
       </c>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
-      <c r="R29" s="4"/>
-      <c r="S29" s="4"/>
-      <c r="T29" s="10"/>
-      <c r="U29" s="11"/>
-      <c r="V29" s="11"/>
-      <c r="W29" s="11"/>
-      <c r="X29" s="11"/>
-      <c r="Y29" s="11"/>
-      <c r="Z29" s="11"/>
-      <c r="AA29" s="12"/>
-      <c r="AB29" s="13"/>
-      <c r="AC29" s="14"/>
+      <c r="R29" s="3"/>
+      <c r="S29" s="3"/>
+      <c r="T29" s="9"/>
+      <c r="U29" s="10"/>
+      <c r="V29" s="10"/>
+      <c r="W29" s="10"/>
+      <c r="X29" s="10"/>
+      <c r="Y29" s="10"/>
+      <c r="Z29" s="10"/>
+      <c r="AA29" s="11"/>
+      <c r="AB29" s="12"/>
+      <c r="AC29" s="13"/>
     </row>
     <row r="30" spans="1:29" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B30" s="1">
         <v>0.106</v>
       </c>
-      <c r="D30" s="16">
+      <c r="D30" s="15">
         <f t="shared" si="0"/>
         <v>4.6243597040409789E-3</v>
       </c>
-      <c r="E30" s="3">
-        <v>28043</v>
-      </c>
-      <c r="F30" s="17">
+      <c r="E30" s="17">
+        <v>44900</v>
+      </c>
+      <c r="F30" s="16">
         <v>281120</v>
       </c>
       <c r="G30" s="2">
@@ -1718,22 +1717,22 @@
       </c>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
-      <c r="R30" s="4"/>
-      <c r="S30" s="4"/>
-      <c r="T30" s="10"/>
-      <c r="U30" s="11"/>
-      <c r="V30" s="11"/>
-      <c r="W30" s="11"/>
-      <c r="X30" s="11"/>
-      <c r="Y30" s="11"/>
-      <c r="Z30" s="11"/>
-      <c r="AA30" s="12"/>
-      <c r="AB30" s="13"/>
-      <c r="AC30" s="14"/>
+      <c r="R30" s="3"/>
+      <c r="S30" s="3"/>
+      <c r="T30" s="9"/>
+      <c r="U30" s="10"/>
+      <c r="V30" s="10"/>
+      <c r="W30" s="10"/>
+      <c r="X30" s="10"/>
+      <c r="Y30" s="10"/>
+      <c r="Z30" s="10"/>
+      <c r="AA30" s="11"/>
+      <c r="AB30" s="12"/>
+      <c r="AC30" s="13"/>
     </row>
     <row r="31" spans="1:29" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B31" s="1">
         <v>8.3000000000000004E-2</v>
@@ -1741,14 +1740,14 @@
       <c r="C31">
         <v>3.52</v>
       </c>
-      <c r="D31" s="16">
+      <c r="D31" s="15">
         <f t="shared" si="0"/>
         <v>8.1891850644153844E-3</v>
       </c>
-      <c r="E31" s="3">
-        <v>29318</v>
-      </c>
-      <c r="F31" s="17">
+      <c r="E31" s="17">
+        <v>46300</v>
+      </c>
+      <c r="F31" s="16">
         <v>268647</v>
       </c>
       <c r="G31" s="2">
@@ -1756,22 +1755,22 @@
       </c>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
-      <c r="R31" s="4"/>
-      <c r="S31" s="4"/>
-      <c r="T31" s="10"/>
-      <c r="U31" s="11"/>
-      <c r="V31" s="11"/>
-      <c r="W31" s="11"/>
-      <c r="X31" s="11"/>
-      <c r="Y31" s="11"/>
-      <c r="Z31" s="11"/>
-      <c r="AA31" s="12"/>
-      <c r="AB31" s="13"/>
-      <c r="AC31" s="14"/>
+      <c r="R31" s="3"/>
+      <c r="S31" s="3"/>
+      <c r="T31" s="9"/>
+      <c r="U31" s="10"/>
+      <c r="V31" s="10"/>
+      <c r="W31" s="10"/>
+      <c r="X31" s="10"/>
+      <c r="Y31" s="10"/>
+      <c r="Z31" s="10"/>
+      <c r="AA31" s="11"/>
+      <c r="AB31" s="12"/>
+      <c r="AC31" s="13"/>
     </row>
     <row r="32" spans="1:29" ht="18" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B32" s="1">
         <v>6.0999999999999999E-2</v>
@@ -1779,14 +1778,14 @@
       <c r="C32">
         <v>3.18</v>
       </c>
-      <c r="D32" s="16">
+      <c r="D32" s="15">
         <f t="shared" si="0"/>
         <v>3.1149648575328347E-3</v>
       </c>
-      <c r="E32" s="3">
-        <v>23143</v>
-      </c>
-      <c r="F32" s="17">
+      <c r="E32" s="17">
+        <v>31000</v>
+      </c>
+      <c r="F32" s="16">
         <v>353134</v>
       </c>
       <c r="G32" s="2">
@@ -1794,37 +1793,37 @@
       </c>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
-      <c r="R32" s="4"/>
-      <c r="S32" s="4"/>
-      <c r="T32" s="10"/>
-      <c r="U32" s="11"/>
-      <c r="V32" s="11"/>
-      <c r="W32" s="11"/>
-      <c r="X32" s="11"/>
-      <c r="Y32" s="11"/>
-      <c r="Z32" s="11"/>
-      <c r="AA32" s="12"/>
-      <c r="AB32" s="13"/>
-      <c r="AC32" s="14"/>
+      <c r="R32" s="3"/>
+      <c r="S32" s="3"/>
+      <c r="T32" s="9"/>
+      <c r="U32" s="10"/>
+      <c r="V32" s="10"/>
+      <c r="W32" s="10"/>
+      <c r="X32" s="10"/>
+      <c r="Y32" s="10"/>
+      <c r="Z32" s="10"/>
+      <c r="AA32" s="11"/>
+      <c r="AB32" s="12"/>
+      <c r="AC32" s="13"/>
     </row>
     <row r="33" spans="1:29" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>35</v>
-      </c>
-      <c r="B33" s="7">
+        <v>34</v>
+      </c>
+      <c r="B33" s="6">
         <v>8.1000000000000003E-2</v>
       </c>
       <c r="C33">
         <v>3.33</v>
       </c>
-      <c r="D33" s="16">
+      <c r="D33" s="15">
         <f t="shared" si="0"/>
         <v>6.1059810432773148E-3</v>
       </c>
-      <c r="E33" s="3">
-        <v>21953</v>
-      </c>
-      <c r="F33" s="17">
+      <c r="E33" s="17">
+        <v>28800</v>
+      </c>
+      <c r="F33" s="16">
         <v>212906</v>
       </c>
       <c r="G33" s="2">
@@ -1832,38 +1831,38 @@
       </c>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
-      <c r="K33" s="6"/>
-      <c r="R33" s="4"/>
-      <c r="S33" s="4"/>
-      <c r="T33" s="10"/>
-      <c r="U33" s="11"/>
-      <c r="V33" s="11"/>
-      <c r="W33" s="11"/>
-      <c r="X33" s="11"/>
-      <c r="Y33" s="11"/>
-      <c r="Z33" s="11"/>
-      <c r="AA33" s="12"/>
-      <c r="AB33" s="13"/>
-      <c r="AC33" s="14"/>
+      <c r="K33" s="5"/>
+      <c r="R33" s="3"/>
+      <c r="S33" s="3"/>
+      <c r="T33" s="9"/>
+      <c r="U33" s="10"/>
+      <c r="V33" s="10"/>
+      <c r="W33" s="10"/>
+      <c r="X33" s="10"/>
+      <c r="Y33" s="10"/>
+      <c r="Z33" s="10"/>
+      <c r="AA33" s="11"/>
+      <c r="AB33" s="12"/>
+      <c r="AC33" s="13"/>
     </row>
     <row r="34" spans="1:29" ht="18" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>17</v>
-      </c>
-      <c r="B34" s="8">
+        <v>16</v>
+      </c>
+      <c r="B34" s="7">
         <v>0.06</v>
       </c>
       <c r="C34">
         <v>3.62</v>
       </c>
-      <c r="D34" s="16">
+      <c r="D34" s="15">
         <f t="shared" si="0"/>
         <v>2.0574015019030965E-2</v>
       </c>
-      <c r="E34" s="3">
-        <v>45436</v>
-      </c>
-      <c r="F34" s="17">
+      <c r="E34" s="17">
+        <v>142000</v>
+      </c>
+      <c r="F34" s="16">
         <v>9721</v>
       </c>
       <c r="G34" s="2">
@@ -1871,18 +1870,18 @@
       </c>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
-      <c r="R34" s="4"/>
-      <c r="S34" s="4"/>
-      <c r="T34" s="10"/>
-      <c r="U34" s="11"/>
-      <c r="V34" s="11"/>
-      <c r="W34" s="11"/>
-      <c r="X34" s="11"/>
-      <c r="Y34" s="11"/>
-      <c r="Z34" s="11"/>
-      <c r="AA34" s="12"/>
-      <c r="AB34" s="13"/>
-      <c r="AC34" s="14"/>
+      <c r="R34" s="3"/>
+      <c r="S34" s="3"/>
+      <c r="T34" s="9"/>
+      <c r="U34" s="10"/>
+      <c r="V34" s="10"/>
+      <c r="W34" s="10"/>
+      <c r="X34" s="10"/>
+      <c r="Y34" s="10"/>
+      <c r="Z34" s="10"/>
+      <c r="AA34" s="11"/>
+      <c r="AB34" s="12"/>
+      <c r="AC34" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>